<commit_message>
agrego ejercicio 2. los outputs deberían ser todos los correctos, faltaría ordenar el código
</commit_message>
<xml_diff>
--- a/tp1/primera_estimacion.xlsx
+++ b/tp1/primera_estimacion.xlsx
@@ -90,715 +90,701 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>320.10696195606266</v>
+        <v>311.99214634304764</v>
       </c>
       <c r="B2" t="n">
-        <v>0.8111391987336849</v>
+        <v>0.9270143532381946</v>
       </c>
       <c r="C2" t="n">
-        <v>0.9431084378186861</v>
+        <v>0.8462265481233605</v>
       </c>
       <c r="D2" t="n">
-        <v>-1.1107584124853722</v>
+        <v>-0.9849226458541296</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>311.99214634304764</v>
+        <v>298.7913801407171</v>
       </c>
       <c r="B3" t="n">
-        <v>0.9270143532381946</v>
+        <v>1.0959254691772786</v>
       </c>
       <c r="C3" t="n">
-        <v>0.8462265481233605</v>
+        <v>0.7990899302380623</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.9849226458541296</v>
+        <v>-0.9469577698084803</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>298.7913801407171</v>
+        <v>286.2289075902831</v>
       </c>
       <c r="B4" t="n">
-        <v>1.0959254691772786</v>
+        <v>1.159249018339312</v>
       </c>
       <c r="C4" t="n">
-        <v>0.7990899302380623</v>
+        <v>1.110745615411233</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.9469577698084803</v>
+        <v>-0.9061621284556703</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>286.2289075902831</v>
+        <v>291.4179754697322</v>
       </c>
       <c r="B5" t="n">
-        <v>1.159249018339312</v>
+        <v>0.9621043745703384</v>
       </c>
       <c r="C5" t="n">
-        <v>1.110745615411233</v>
+        <v>1.1519077441167456</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.9061621284556703</v>
+        <v>-0.9667734305408507</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>291.4179754697322</v>
+        <v>293.03812414644483</v>
       </c>
       <c r="B6" t="n">
-        <v>0.9621043745703384</v>
+        <v>0.7872343314300287</v>
       </c>
       <c r="C6" t="n">
-        <v>1.1519077441167456</v>
+        <v>1.0303513519079783</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.9667734305408507</v>
+        <v>-0.7413380768974539</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>293.03812414644483</v>
+        <v>263.5973280763877</v>
       </c>
       <c r="B7" t="n">
-        <v>0.7872343314300287</v>
+        <v>1.1497489342092988</v>
       </c>
       <c r="C7" t="n">
-        <v>1.0303513519079783</v>
+        <v>1.166393538649101</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.7413380768974539</v>
+        <v>-0.6387484606688087</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>263.5973280763877</v>
+        <v>312.1813869669151</v>
       </c>
       <c r="B8" t="n">
-        <v>1.1497489342092988</v>
+        <v>0.9517961709339885</v>
       </c>
       <c r="C8" t="n">
-        <v>1.166393538649101</v>
+        <v>0.8146379132550743</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.6387484606688087</v>
+        <v>-1.0462144752287337</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>312.1813869669151</v>
+        <v>297.0430955798718</v>
       </c>
       <c r="B9" t="n">
-        <v>0.9517961709339885</v>
+        <v>0.9812010230672212</v>
       </c>
       <c r="C9" t="n">
-        <v>0.8146379132550743</v>
+        <v>1.0446316485376108</v>
       </c>
       <c r="D9" t="n">
-        <v>-1.0462144752287337</v>
+        <v>-0.9124796047127766</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>297.0430955798718</v>
+        <v>307.89411205938046</v>
       </c>
       <c r="B10" t="n">
-        <v>0.9812010230672212</v>
+        <v>0.7765950841122121</v>
       </c>
       <c r="C10" t="n">
-        <v>1.0446316485376108</v>
+        <v>0.9667612940375263</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.9124796047127766</v>
+        <v>-0.9465462959506593</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>307.89411205938046</v>
+        <v>311.8210807979068</v>
       </c>
       <c r="B11" t="n">
-        <v>0.7765950841122121</v>
+        <v>1.1071226149492261</v>
       </c>
       <c r="C11" t="n">
-        <v>0.9667612940375263</v>
+        <v>0.8586009975145162</v>
       </c>
       <c r="D11" t="n">
-        <v>-0.9465462959506593</v>
+        <v>-1.2671868163985485</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>311.8210807979068</v>
+        <v>299.9003787613883</v>
       </c>
       <c r="B12" t="n">
-        <v>1.1071226149492261</v>
+        <v>0.9396498790816799</v>
       </c>
       <c r="C12" t="n">
-        <v>0.8586009975145162</v>
+        <v>0.9428621956792989</v>
       </c>
       <c r="D12" t="n">
-        <v>-1.2671868163985485</v>
+        <v>-0.9989236288321327</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>299.9003787613883</v>
+        <v>299.43586673644734</v>
       </c>
       <c r="B13" t="n">
-        <v>0.9396498790816799</v>
+        <v>1.1706816918099097</v>
       </c>
       <c r="C13" t="n">
-        <v>0.9428621956792989</v>
+        <v>1.0533212715120828</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.9989236288321327</v>
+        <v>-1.1769847846570622</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>299.43586673644734</v>
+        <v>313.49809981002846</v>
       </c>
       <c r="B14" t="n">
-        <v>1.1706816918099097</v>
+        <v>0.890576637870783</v>
       </c>
       <c r="C14" t="n">
-        <v>1.0533212715120828</v>
+        <v>0.9416103465467662</v>
       </c>
       <c r="D14" t="n">
-        <v>-1.1769847846570622</v>
+        <v>-1.0657817005403543</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>313.49809981002846</v>
+        <v>287.1120274375085</v>
       </c>
       <c r="B15" t="n">
-        <v>0.890576637870783</v>
+        <v>0.9946128733185879</v>
       </c>
       <c r="C15" t="n">
-        <v>0.9416103465467662</v>
+        <v>1.2511086692703715</v>
       </c>
       <c r="D15" t="n">
-        <v>-1.0657817005403543</v>
+        <v>-1.0027557587433895</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>287.1120274375085</v>
+        <v>285.0851308004906</v>
       </c>
       <c r="B16" t="n">
-        <v>0.9946128733185879</v>
+        <v>1.1049534416558067</v>
       </c>
       <c r="C16" t="n">
-        <v>1.2511086692703715</v>
+        <v>1.071995667874754</v>
       </c>
       <c r="D16" t="n">
-        <v>-1.0027557587433895</v>
+        <v>-0.9688289046899833</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>285.0851308004906</v>
+        <v>300.557957373688</v>
       </c>
       <c r="B17" t="n">
-        <v>1.1049534416558067</v>
+        <v>0.8917939168345853</v>
       </c>
       <c r="C17" t="n">
-        <v>1.071995667874754</v>
+        <v>0.9474738053107582</v>
       </c>
       <c r="D17" t="n">
-        <v>-0.9688289046899833</v>
+        <v>-0.9786974471296049</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>300.557957373688</v>
+        <v>290.9302891432309</v>
       </c>
       <c r="B18" t="n">
-        <v>0.8917939168345853</v>
+        <v>0.8712283838919981</v>
       </c>
       <c r="C18" t="n">
-        <v>0.9474738053107582</v>
+        <v>0.963883147460799</v>
       </c>
       <c r="D18" t="n">
-        <v>-0.9786974471296049</v>
+        <v>-0.7024367203724046</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>290.9302891432309</v>
+        <v>298.59873858853734</v>
       </c>
       <c r="B19" t="n">
-        <v>0.8712283838919981</v>
+        <v>1.2240110654328622</v>
       </c>
       <c r="C19" t="n">
-        <v>0.963883147460799</v>
+        <v>0.9374271834326655</v>
       </c>
       <c r="D19" t="n">
-        <v>-0.7024367203724046</v>
+        <v>-1.0220266078304612</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>298.59873858853734</v>
+        <v>329.7271238288696</v>
       </c>
       <c r="B20" t="n">
-        <v>1.2240110654328622</v>
+        <v>0.9339849020859703</v>
       </c>
       <c r="C20" t="n">
-        <v>0.9374271834326655</v>
+        <v>0.7239021343939431</v>
       </c>
       <c r="D20" t="n">
-        <v>-1.0220266078304612</v>
+        <v>-1.2088741780288128</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>329.7271238288696</v>
+        <v>312.3787506891291</v>
       </c>
       <c r="B21" t="n">
-        <v>0.9339849020859703</v>
+        <v>0.9727275962733406</v>
       </c>
       <c r="C21" t="n">
-        <v>0.7239021343939431</v>
+        <v>0.9014241956585107</v>
       </c>
       <c r="D21" t="n">
-        <v>-1.2088741780288128</v>
+        <v>-1.0407043023511073</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>312.3787506891291</v>
+        <v>295.53738372473646</v>
       </c>
       <c r="B22" t="n">
-        <v>0.9727275962733406</v>
+        <v>1.052415254157812</v>
       </c>
       <c r="C22" t="n">
-        <v>0.9014241956585107</v>
+        <v>1.0083267833431595</v>
       </c>
       <c r="D22" t="n">
-        <v>-1.0407043023511073</v>
+        <v>-0.9889734357274239</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>295.53738372473646</v>
+        <v>288.5435092335864</v>
       </c>
       <c r="B23" t="n">
-        <v>1.052415254157812</v>
+        <v>0.9941206270174264</v>
       </c>
       <c r="C23" t="n">
-        <v>1.0083267833431595</v>
+        <v>1.0309076585694699</v>
       </c>
       <c r="D23" t="n">
-        <v>-0.9889734357274239</v>
+        <v>-0.8296961970412741</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>288.5435092335864</v>
+        <v>283.0184035049843</v>
       </c>
       <c r="B24" t="n">
-        <v>0.9941206270174264</v>
+        <v>1.2884707941108466</v>
       </c>
       <c r="C24" t="n">
-        <v>1.0309076585694699</v>
+        <v>1.1993307567603357</v>
       </c>
       <c r="D24" t="n">
-        <v>-0.8296961970412741</v>
+        <v>-1.0149998564150353</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>283.0184035049843</v>
+        <v>293.6629293110402</v>
       </c>
       <c r="B25" t="n">
-        <v>1.2884707941108466</v>
+        <v>0.9714897078366969</v>
       </c>
       <c r="C25" t="n">
-        <v>1.1993307567603357</v>
+        <v>1.1426063557779298</v>
       </c>
       <c r="D25" t="n">
-        <v>-1.0149998564150353</v>
+        <v>-1.1496407613956727</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>293.6629293110402</v>
+        <v>312.877097806259</v>
       </c>
       <c r="B26" t="n">
-        <v>0.9714897078366969</v>
+        <v>1.0434242051140201</v>
       </c>
       <c r="C26" t="n">
-        <v>1.1426063557779298</v>
+        <v>0.6911478224152651</v>
       </c>
       <c r="D26" t="n">
-        <v>-1.1496407613956727</v>
+        <v>-1.0364044018452898</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>312.877097806259</v>
+        <v>291.8811812193485</v>
       </c>
       <c r="B27" t="n">
-        <v>1.0434242051140201</v>
+        <v>0.936543569008261</v>
       </c>
       <c r="C27" t="n">
-        <v>0.6911478224152651</v>
+        <v>1.1241338513651689</v>
       </c>
       <c r="D27" t="n">
-        <v>-1.0364044018452898</v>
+        <v>-0.8240959236683244</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>291.8811812193485</v>
+        <v>271.8174322206766</v>
       </c>
       <c r="B28" t="n">
-        <v>0.936543569008261</v>
+        <v>1.1247112051151047</v>
       </c>
       <c r="C28" t="n">
-        <v>1.1241338513651689</v>
+        <v>0.9627424393251375</v>
       </c>
       <c r="D28" t="n">
-        <v>-0.8240959236683244</v>
+        <v>-0.6040162297333513</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>271.8174322206766</v>
+        <v>316.0871161740264</v>
       </c>
       <c r="B29" t="n">
-        <v>1.1247112051151047</v>
+        <v>0.953335516408614</v>
       </c>
       <c r="C29" t="n">
-        <v>0.9627424393251375</v>
+        <v>0.8401971547489173</v>
       </c>
       <c r="D29" t="n">
-        <v>-0.6040162297333513</v>
+        <v>-1.0844335179321731</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>316.0871161740264</v>
+        <v>317.0561730419182</v>
       </c>
       <c r="B30" t="n">
-        <v>0.953335516408614</v>
+        <v>1.0910878823532777</v>
       </c>
       <c r="C30" t="n">
-        <v>0.8401971547489173</v>
+        <v>0.9901735273832584</v>
       </c>
       <c r="D30" t="n">
-        <v>-1.0844335179321731</v>
+        <v>-1.3244641047803258</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>317.0561730419182</v>
+        <v>303.5247184386089</v>
       </c>
       <c r="B31" t="n">
-        <v>1.0910878823532777</v>
+        <v>0.9438193966403764</v>
       </c>
       <c r="C31" t="n">
-        <v>0.9901735273832584</v>
+        <v>1.0017870092189205</v>
       </c>
       <c r="D31" t="n">
-        <v>-1.3244641047803258</v>
+        <v>-0.9079280818439439</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>303.5247184386089</v>
+        <v>322.06222679530634</v>
       </c>
       <c r="B32" t="n">
-        <v>0.9438193966403764</v>
+        <v>0.701384746806264</v>
       </c>
       <c r="C32" t="n">
-        <v>1.0017870092189205</v>
+        <v>1.1688533013791396</v>
       </c>
       <c r="D32" t="n">
-        <v>-0.9079280818439439</v>
+        <v>-1.2829202247391114</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>322.06222679530634</v>
+        <v>304.1762768687312</v>
       </c>
       <c r="B33" t="n">
-        <v>0.701384746806264</v>
+        <v>1.1109803872994486</v>
       </c>
       <c r="C33" t="n">
-        <v>1.1688533013791396</v>
+        <v>0.7707441051976587</v>
       </c>
       <c r="D33" t="n">
-        <v>-1.2829202247391114</v>
+        <v>-0.9789319070909143</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>304.1762768687312</v>
+        <v>285.6311234833858</v>
       </c>
       <c r="B34" t="n">
-        <v>1.1109803872994486</v>
+        <v>1.2404354955876042</v>
       </c>
       <c r="C34" t="n">
-        <v>0.7707441051976587</v>
+        <v>1.1969589622933947</v>
       </c>
       <c r="D34" t="n">
-        <v>-0.9789319070909143</v>
+        <v>-1.2502849126735123</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>285.6311234833858</v>
+        <v>303.06031491229794</v>
       </c>
       <c r="B35" t="n">
-        <v>1.2404354955876042</v>
+        <v>0.888217064219625</v>
       </c>
       <c r="C35" t="n">
-        <v>1.1969589622933947</v>
+        <v>1.0763221310728708</v>
       </c>
       <c r="D35" t="n">
-        <v>-1.2502849126735123</v>
+        <v>-1.0560560398835144</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>303.06031491229794</v>
+        <v>285.13049535497083</v>
       </c>
       <c r="B36" t="n">
-        <v>0.888217064219625</v>
+        <v>0.7923322984031214</v>
       </c>
       <c r="C36" t="n">
-        <v>1.0763221310728708</v>
+        <v>1.149921660413218</v>
       </c>
       <c r="D36" t="n">
-        <v>-1.0560560398835144</v>
+        <v>-0.7378349901171753</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>285.13049535497083</v>
+        <v>296.25055184439765</v>
       </c>
       <c r="B37" t="n">
-        <v>0.7923322984031214</v>
+        <v>0.7925103373412506</v>
       </c>
       <c r="C37" t="n">
-        <v>1.149921660413218</v>
+        <v>1.0087361172006482</v>
       </c>
       <c r="D37" t="n">
-        <v>-0.7378349901171753</v>
+        <v>-0.7663486709926336</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>296.25055184439765</v>
+        <v>309.00499198577427</v>
       </c>
       <c r="B38" t="n">
-        <v>0.7925103373412506</v>
+        <v>0.9763503018508437</v>
       </c>
       <c r="C38" t="n">
-        <v>1.0087361172006482</v>
+        <v>0.9121540582154886</v>
       </c>
       <c r="D38" t="n">
-        <v>-0.7663486709926336</v>
+        <v>-1.0796912124988454</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>309.00499198577427</v>
+        <v>287.4716142005602</v>
       </c>
       <c r="B39" t="n">
-        <v>0.9763503018508437</v>
+        <v>1.2246963892159897</v>
       </c>
       <c r="C39" t="n">
-        <v>0.9121540582154886</v>
+        <v>1.1197114829755035</v>
       </c>
       <c r="D39" t="n">
-        <v>-1.0796912124988454</v>
+        <v>-1.1142019695553311</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>287.4716142005602</v>
+        <v>294.28734340928077</v>
       </c>
       <c r="B40" t="n">
-        <v>1.2246963892159897</v>
+        <v>1.0973313440156138</v>
       </c>
       <c r="C40" t="n">
-        <v>1.1197114829755035</v>
+        <v>0.9515269540794511</v>
       </c>
       <c r="D40" t="n">
-        <v>-1.1142019695553311</v>
+        <v>-0.9463849456494806</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>294.28734340928077</v>
+        <v>294.53479933654717</v>
       </c>
       <c r="B41" t="n">
-        <v>1.0973313440156138</v>
+        <v>0.9937736745431772</v>
       </c>
       <c r="C41" t="n">
-        <v>0.9515269540794511</v>
+        <v>0.9692114121915836</v>
       </c>
       <c r="D41" t="n">
-        <v>-0.9463849456494806</v>
+        <v>-0.9663366485129243</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>294.53479933654717</v>
+        <v>307.7189000628035</v>
       </c>
       <c r="B42" t="n">
-        <v>0.9937736745431772</v>
+        <v>0.9557686993055949</v>
       </c>
       <c r="C42" t="n">
-        <v>0.9692114121915836</v>
+        <v>0.8755685256087914</v>
       </c>
       <c r="D42" t="n">
-        <v>-0.9663366485129243</v>
+        <v>-0.9785422795598073</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>307.7189000628035</v>
+        <v>305.29109761143064</v>
       </c>
       <c r="B43" t="n">
-        <v>0.9557686993055949</v>
+        <v>1.0275213845520386</v>
       </c>
       <c r="C43" t="n">
-        <v>0.8755685256087914</v>
+        <v>0.8133136291506268</v>
       </c>
       <c r="D43" t="n">
-        <v>-0.9785422795598073</v>
+        <v>-0.8067139652616918</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>305.29109761143064</v>
+        <v>293.9985582250761</v>
       </c>
       <c r="B44" t="n">
-        <v>1.0275213845520386</v>
+        <v>0.8753816941849231</v>
       </c>
       <c r="C44" t="n">
-        <v>0.8133136291506268</v>
+        <v>1.0954283913771563</v>
       </c>
       <c r="D44" t="n">
-        <v>-0.8067139652616918</v>
+        <v>-0.8267968167768436</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>293.9985582250761</v>
+        <v>302.40608696088464</v>
       </c>
       <c r="B45" t="n">
-        <v>0.8753816941849231</v>
+        <v>0.92326684778669</v>
       </c>
       <c r="C45" t="n">
-        <v>1.0954283913771563</v>
+        <v>0.9652550945952517</v>
       </c>
       <c r="D45" t="n">
-        <v>-0.8267968167768436</v>
+        <v>-0.9920607042160513</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>302.40608696088464</v>
+        <v>287.40024546417607</v>
       </c>
       <c r="B46" t="n">
-        <v>0.92326684778669</v>
+        <v>1.0206215198743904</v>
       </c>
       <c r="C46" t="n">
-        <v>0.9652550945952517</v>
+        <v>1.2903176177040958</v>
       </c>
       <c r="D46" t="n">
-        <v>-0.9920607042160513</v>
+        <v>-1.0269655536390125</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>287.40024546417607</v>
+        <v>320.10696195606266</v>
       </c>
       <c r="B47" t="n">
-        <v>1.0206215198743904</v>
+        <v>0.8111391987336849</v>
       </c>
       <c r="C47" t="n">
-        <v>1.2903176177040958</v>
+        <v>0.9431084378186861</v>
       </c>
       <c r="D47" t="n">
-        <v>-1.0269655536390125</v>
+        <v>-1.1107584124853722</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>320.10696195606266</v>
+        <v>289.8211262164983</v>
       </c>
       <c r="B48" t="n">
-        <v>0.8111391987336849</v>
+        <v>0.955674998898326</v>
       </c>
       <c r="C48" t="n">
-        <v>0.9431084378186861</v>
+        <v>1.0990568180847404</v>
       </c>
       <c r="D48" t="n">
-        <v>-1.1107584124853722</v>
+        <v>-0.9273559294144769</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>289.8211262164983</v>
+        <v>291.35444062132626</v>
       </c>
       <c r="B49" t="n">
-        <v>0.955674998898326</v>
+        <v>0.8810652275985587</v>
       </c>
       <c r="C49" t="n">
-        <v>1.0990568180847404</v>
+        <v>1.0313051447420043</v>
       </c>
       <c r="D49" t="n">
-        <v>-0.9273559294144769</v>
+        <v>-0.7430049279837965</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>291.35444062132626</v>
+        <v>303.18132989573525</v>
       </c>
       <c r="B50" t="n">
-        <v>0.8810652275985587</v>
+        <v>0.9876189567964386</v>
       </c>
       <c r="C50" t="n">
-        <v>1.0313051447420043</v>
+        <v>1.1048135969303368</v>
       </c>
       <c r="D50" t="n">
-        <v>-0.7430049279837965</v>
+        <v>-1.1316079247140394</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>303.18132989573525</v>
+        <v>298.82746384813186</v>
       </c>
       <c r="B51" t="n">
-        <v>0.9876189567964386</v>
+        <v>0.8829291781292657</v>
       </c>
       <c r="C51" t="n">
-        <v>1.1048135969303368</v>
+        <v>1.0760826512624435</v>
       </c>
       <c r="D51" t="n">
-        <v>-1.1316079247140394</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="n">
-        <v>298.82746384813186</v>
-      </c>
-      <c r="B52" t="n">
-        <v>0.8829291781292657</v>
-      </c>
-      <c r="C52" t="n">
-        <v>1.0760826512624435</v>
-      </c>
-      <c r="D52" t="n">
         <v>-1.0475734619910977</v>
       </c>
     </row>

</xml_diff>